<commit_message>
code review please rework
</commit_message>
<xml_diff>
--- a/tests/artifact/script/Export-Import.xlsx
+++ b/tests/artifact/script/Export-Import.xlsx
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1417" uniqueCount="840">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="842">
   <si>
     <t>target</t>
   </si>
@@ -2333,6 +2333,9 @@
     <t>[JSON(${response}.body) =&gt; extract(token)]</t>
   </si>
   <si>
+    <t>remove the commented code if not required?</t>
+  </si>
+  <si>
     <t>$(projectfile|macro|${gnukhata.path}|MacroLibrary|getGKToken)</t>
   </si>
   <si>
@@ -2380,6 +2383,9 @@
   </si>
   <si>
     <t>response</t>
+  </si>
+  <si>
+    <t>why the code is in red color and commented?</t>
   </si>
   <si>
     <t>And I save the Gk Version of the response</t>
@@ -2671,7 +2677,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="35">
+  <fonts count="36">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2736,6 +2742,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Consolas"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Tahoma"/>
       <charset val="134"/>
     </font>
     <font>
@@ -3284,14 +3297,11 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3300,119 +3310,122 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3585,19 +3598,23 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -3609,7 +3626,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
@@ -3622,7 +3639,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -3639,22 +3656,22 @@
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -6700,7 +6717,7 @@
   <dimension ref="A1:XFD195"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
@@ -6834,7 +6851,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="5" s="53" customFormat="1" ht="32" customHeight="1" spans="1:16384">
+    <row r="5" s="54" customFormat="1" ht="32" customHeight="1" spans="1:16384">
       <c r="A5" s="18" t="s">
         <v>747</v>
       </c>
@@ -23239,16 +23256,16 @@
       <c r="B6" s="3" t="s">
         <v>752</v>
       </c>
-      <c r="C6" s="56" t="s">
+      <c r="C6" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="57" t="s">
+      <c r="D6" s="58" t="s">
         <v>471</v>
       </c>
-      <c r="E6" s="57" t="s">
+      <c r="E6" s="58" t="s">
         <v>753</v>
       </c>
-      <c r="F6" s="58" t="s">
+      <c r="F6" s="59" t="s">
         <v>754</v>
       </c>
       <c r="G6" s="29"/>
@@ -23262,7 +23279,9 @@
       <c r="O6" s="21"/>
     </row>
     <row r="7" s="10" customFormat="1" ht="42" customHeight="1" spans="1:15">
-      <c r="A7" s="18"/>
+      <c r="A7" s="48" t="s">
+        <v>755</v>
+      </c>
       <c r="B7" s="19"/>
       <c r="C7" s="28" t="s">
         <v>5</v>
@@ -23271,10 +23290,10 @@
         <v>447</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="F7" s="43" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="G7" s="29" t="s">
         <v>751</v>
@@ -23291,16 +23310,16 @@
     <row r="8" s="10" customFormat="1" spans="1:15">
       <c r="A8" s="18"/>
       <c r="B8" s="19"/>
-      <c r="C8" s="56" t="s">
+      <c r="C8" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="57" t="s">
+      <c r="D8" s="58" t="s">
         <v>471</v>
       </c>
-      <c r="E8" s="57" t="s">
-        <v>757</v>
-      </c>
-      <c r="F8" s="58" t="s">
+      <c r="E8" s="58" t="s">
+        <v>758</v>
+      </c>
+      <c r="F8" s="59" t="s">
         <v>754</v>
       </c>
       <c r="G8" s="29"/>
@@ -23313,7 +23332,7 @@
       <c r="N8" s="22"/>
       <c r="O8" s="21"/>
     </row>
-    <row r="9" s="54" customFormat="1" ht="29" spans="1:15">
+    <row r="9" s="55" customFormat="1" ht="29" spans="1:15">
       <c r="A9" s="18"/>
       <c r="B9" s="19"/>
       <c r="C9" s="28" t="s">
@@ -23326,7 +23345,7 @@
         <v>753</v>
       </c>
       <c r="F9" s="43" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="H9" s="25"/>
       <c r="I9" s="25"/>
@@ -23337,7 +23356,7 @@
       <c r="N9" s="22"/>
       <c r="O9" s="21"/>
     </row>
-    <row r="10" s="54" customFormat="1" ht="29" spans="1:15">
+    <row r="10" s="55" customFormat="1" ht="29" spans="1:15">
       <c r="A10" s="18"/>
       <c r="B10" s="19"/>
       <c r="C10" s="28" t="s">
@@ -23347,10 +23366,10 @@
         <v>471</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="F10" s="43" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="G10" s="29"/>
       <c r="H10" s="25"/>
@@ -23378,73 +23397,73 @@
       <c r="N11" s="22"/>
       <c r="O11" s="21"/>
     </row>
-    <row r="12" s="55" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A12" s="59"/>
-      <c r="B12" s="49"/>
-      <c r="C12" s="60"/>
-      <c r="D12" s="61"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="61"/>
+    <row r="12" s="56" customFormat="1" ht="23" customHeight="1" spans="1:15">
+      <c r="A12" s="60"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="62"/>
       <c r="H12" s="41"/>
       <c r="I12" s="41"/>
-      <c r="J12" s="65"/>
-      <c r="K12" s="66"/>
-      <c r="L12" s="67"/>
-      <c r="M12" s="68"/>
-      <c r="N12" s="67"/>
-      <c r="O12" s="66"/>
-    </row>
-    <row r="13" s="55" customFormat="1" ht="19" customHeight="1" spans="1:15">
-      <c r="A13" s="59"/>
-      <c r="B13" s="49"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="61"/>
+      <c r="J12" s="66"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="68"/>
+      <c r="M12" s="69"/>
+      <c r="N12" s="68"/>
+      <c r="O12" s="67"/>
+    </row>
+    <row r="13" s="56" customFormat="1" ht="19" customHeight="1" spans="1:15">
+      <c r="A13" s="60"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="62"/>
       <c r="H13" s="41"/>
       <c r="I13" s="41"/>
-      <c r="J13" s="65"/>
-      <c r="K13" s="66"/>
-      <c r="L13" s="67"/>
-      <c r="M13" s="68"/>
-      <c r="N13" s="67"/>
-      <c r="O13" s="66"/>
-    </row>
-    <row r="14" s="55" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A14" s="59"/>
-      <c r="B14" s="49"/>
-      <c r="C14" s="63"/>
+      <c r="J13" s="66"/>
+      <c r="K13" s="67"/>
+      <c r="L13" s="68"/>
+      <c r="M13" s="69"/>
+      <c r="N13" s="68"/>
+      <c r="O13" s="67"/>
+    </row>
+    <row r="14" s="56" customFormat="1" ht="23" customHeight="1" spans="1:15">
+      <c r="A14" s="60"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="64"/>
       <c r="D14" s="41"/>
       <c r="E14" s="41"/>
       <c r="F14" s="41"/>
       <c r="G14" s="41"/>
       <c r="H14" s="41"/>
       <c r="I14" s="41"/>
-      <c r="J14" s="65"/>
-      <c r="K14" s="66"/>
-      <c r="L14" s="67"/>
-      <c r="M14" s="68"/>
-      <c r="N14" s="67"/>
-      <c r="O14" s="66"/>
-    </row>
-    <row r="15" s="55" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A15" s="59"/>
-      <c r="B15" s="49"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="58"/>
+      <c r="J14" s="66"/>
+      <c r="K14" s="67"/>
+      <c r="L14" s="68"/>
+      <c r="M14" s="69"/>
+      <c r="N14" s="68"/>
+      <c r="O14" s="67"/>
+    </row>
+    <row r="15" s="56" customFormat="1" ht="23" customHeight="1" spans="1:15">
+      <c r="A15" s="60"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="58"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="59"/>
       <c r="G15" s="41"/>
       <c r="H15" s="41"/>
       <c r="I15" s="41"/>
-      <c r="J15" s="65"/>
-      <c r="K15" s="66"/>
-      <c r="L15" s="67"/>
-      <c r="M15" s="68"/>
-      <c r="N15" s="67"/>
-      <c r="O15" s="66"/>
+      <c r="J15" s="66"/>
+      <c r="K15" s="67"/>
+      <c r="L15" s="68"/>
+      <c r="M15" s="69"/>
+      <c r="N15" s="68"/>
+      <c r="O15" s="67"/>
     </row>
     <row r="16" s="10" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A16" s="18"/>
@@ -23567,7 +23586,7 @@
     </row>
     <row r="23" s="10" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A23" s="18"/>
-      <c r="B23" s="64"/>
+      <c r="B23" s="65"/>
       <c r="C23" s="24"/>
       <c r="D23" s="25"/>
       <c r="E23" s="25"/>
@@ -26564,8 +26583,8 @@
   <sheetPr/>
   <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
@@ -26619,7 +26638,7 @@
     </row>
     <row r="2" s="10" customFormat="1" ht="93" customHeight="1" spans="1:15">
       <c r="A2" s="14" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
@@ -26629,7 +26648,7 @@
       <c r="G2" s="16"/>
       <c r="H2" s="16"/>
       <c r="I2" s="17" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="J2" s="31"/>
       <c r="K2" s="21"/>
@@ -26702,10 +26721,10 @@
     </row>
     <row r="5" s="10" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A5" s="18" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="C5" s="28" t="s">
         <v>35</v>
@@ -26714,10 +26733,10 @@
         <v>263</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="F5" s="29" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="G5" s="25"/>
       <c r="H5" s="25"/>
@@ -26732,7 +26751,7 @@
     <row r="6" s="10" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A6" s="18"/>
       <c r="B6" s="21" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="C6" s="24" t="s">
         <v>5</v>
@@ -26741,10 +26760,10 @@
         <v>471</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="F6" s="26" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="G6" s="25"/>
       <c r="H6" s="25"/>
@@ -26759,7 +26778,7 @@
     <row r="7" s="10" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A7" s="18"/>
       <c r="B7" s="21" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="C7" s="24" t="s">
         <v>35</v>
@@ -26768,11 +26787,11 @@
         <v>197</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="F7" s="25"/>
       <c r="G7" s="25" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="H7" s="25"/>
       <c r="I7" s="25"/>
@@ -26784,21 +26803,23 @@
       <c r="O7" s="21"/>
     </row>
     <row r="8" s="10" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A8" s="18"/>
+      <c r="A8" s="48" t="s">
+        <v>772</v>
+      </c>
       <c r="B8" s="19" t="s">
-        <v>771</v>
-      </c>
-      <c r="C8" s="48" t="s">
+        <v>773</v>
+      </c>
+      <c r="C8" s="49" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="30" t="s">
         <v>471</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
       <c r="F8" s="30" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="G8" s="25"/>
       <c r="H8" s="25"/>
@@ -26820,10 +26841,10 @@
         <v>447</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="F9" s="26" t="s">
-        <v>775</v>
+        <v>777</v>
       </c>
       <c r="G9" s="25"/>
       <c r="H9" s="25"/>
@@ -26838,19 +26859,19 @@
     <row r="10" s="10" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A10" s="18"/>
       <c r="B10" s="19" t="s">
-        <v>776</v>
-      </c>
-      <c r="C10" s="48" t="s">
+        <v>778</v>
+      </c>
+      <c r="C10" s="49" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="30" t="s">
         <v>49</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="F10" s="30" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
       <c r="G10" s="25"/>
       <c r="H10" s="25"/>
@@ -26865,7 +26886,7 @@
     <row r="11" s="10" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A11" s="18"/>
       <c r="B11" s="19" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
       <c r="C11" s="28" t="s">
         <v>35</v>
@@ -26874,7 +26895,7 @@
         <v>107</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="F11" s="47"/>
       <c r="G11" s="29"/>
@@ -26889,10 +26910,10 @@
     </row>
     <row r="12" s="10" customFormat="1" ht="42" customHeight="1" spans="1:15">
       <c r="A12" s="18" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="C12" s="28" t="s">
         <v>35</v>
@@ -26901,10 +26922,10 @@
         <v>263</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="F12" s="29" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
@@ -26919,7 +26940,7 @@
     <row r="13" s="10" customFormat="1" ht="42" customHeight="1" spans="1:15">
       <c r="A13" s="18"/>
       <c r="B13" s="19" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="C13" s="24" t="s">
         <v>5</v>
@@ -26928,10 +26949,10 @@
         <v>471</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="F13" s="26" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="G13" s="25"/>
       <c r="H13" s="25"/>
@@ -26946,7 +26967,7 @@
     <row r="14" s="10" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A14" s="18"/>
       <c r="B14" s="19" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="C14" s="24" t="s">
         <v>35</v>
@@ -26955,11 +26976,11 @@
         <v>197</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="F14" s="25"/>
       <c r="G14" s="25" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="H14" s="25"/>
       <c r="I14" s="25"/>
@@ -26972,20 +26993,20 @@
     </row>
     <row r="15" s="10" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A15" s="18"/>
-      <c r="B15" s="49" t="s">
-        <v>783</v>
-      </c>
-      <c r="C15" s="50" t="s">
+      <c r="B15" s="50" t="s">
+        <v>785</v>
+      </c>
+      <c r="C15" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="51" t="s">
+      <c r="D15" s="52" t="s">
         <v>471</v>
       </c>
-      <c r="E15" s="51" t="s">
-        <v>784</v>
-      </c>
-      <c r="F15" s="51" t="s">
-        <v>785</v>
+      <c r="E15" s="52" t="s">
+        <v>786</v>
+      </c>
+      <c r="F15" s="52" t="s">
+        <v>787</v>
       </c>
       <c r="G15" s="25"/>
       <c r="H15" s="25"/>
@@ -27000,17 +27021,17 @@
     <row r="16" s="10" customFormat="1" ht="157" customHeight="1" spans="1:15">
       <c r="A16" s="18"/>
       <c r="B16" s="19"/>
-      <c r="C16" s="48" t="s">
+      <c r="C16" s="49" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="30" t="s">
         <v>447</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>774</v>
-      </c>
-      <c r="F16" s="52" t="s">
-        <v>786</v>
+        <v>776</v>
+      </c>
+      <c r="F16" s="53" t="s">
+        <v>788</v>
       </c>
       <c r="G16" s="25"/>
       <c r="H16" s="25"/>
@@ -27024,20 +27045,20 @@
     </row>
     <row r="17" s="10" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A17" s="18"/>
-      <c r="B17" s="49" t="s">
-        <v>776</v>
-      </c>
-      <c r="C17" s="50" t="s">
+      <c r="B17" s="50" t="s">
+        <v>778</v>
+      </c>
+      <c r="C17" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="51" t="s">
+      <c r="D17" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="E17" s="51" t="s">
-        <v>787</v>
-      </c>
-      <c r="F17" s="51" t="s">
-        <v>788</v>
+      <c r="E17" s="52" t="s">
+        <v>789</v>
+      </c>
+      <c r="F17" s="52" t="s">
+        <v>790</v>
       </c>
       <c r="G17" s="25"/>
       <c r="H17" s="25"/>
@@ -27052,7 +27073,7 @@
     <row r="18" s="10" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A18" s="18"/>
       <c r="B18" s="42" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
       <c r="C18" s="28" t="s">
         <v>35</v>
@@ -27061,7 +27082,7 @@
         <v>107</v>
       </c>
       <c r="E18" s="29" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="F18" s="47"/>
       <c r="G18" s="29"/>
@@ -28005,7 +28026,7 @@
   <sheetPr/>
   <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="C3" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="A57" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -28060,7 +28081,7 @@
     </row>
     <row r="2" s="10" customFormat="1" ht="93" customHeight="1" spans="1:15">
       <c r="A2" s="14" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
@@ -28070,7 +28091,7 @@
       <c r="G2" s="16"/>
       <c r="H2" s="16"/>
       <c r="I2" s="17" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="J2" s="31"/>
       <c r="K2" s="21"/>
@@ -28143,10 +28164,10 @@
     </row>
     <row r="5" s="10" customFormat="1" ht="40" customHeight="1" spans="1:15">
       <c r="A5" s="18" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="C5" s="24" t="s">
         <v>5</v>
@@ -28155,10 +28176,10 @@
         <v>471</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="G5" s="25"/>
       <c r="H5" s="25"/>
@@ -28173,7 +28194,7 @@
     <row r="6" s="10" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A6" s="18"/>
       <c r="B6" s="19" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="C6" s="24" t="s">
         <v>35</v>
@@ -28182,11 +28203,11 @@
         <v>197</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="F6" s="25"/>
       <c r="G6" s="25" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="H6" s="25"/>
       <c r="I6" s="25"/>
@@ -28207,7 +28228,7 @@
         <v>536</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>790</v>
+        <v>792</v>
       </c>
       <c r="F7" s="25"/>
       <c r="G7" s="25"/>
@@ -28223,7 +28244,7 @@
     <row r="8" s="10" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A8" s="18"/>
       <c r="B8" s="19" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="C8" s="24" t="s">
         <v>5</v>
@@ -28232,10 +28253,10 @@
         <v>471</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="G8" s="25"/>
       <c r="H8" s="25"/>
@@ -28257,10 +28278,10 @@
         <v>447</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="F9" s="26" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
       <c r="G9" s="25"/>
       <c r="H9" s="25"/>
@@ -28275,7 +28296,7 @@
     <row r="10" s="10" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A10" s="18"/>
       <c r="B10" s="19" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
       <c r="C10" s="24" t="s">
         <v>5</v>
@@ -28284,10 +28305,10 @@
         <v>49</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>792</v>
+        <v>794</v>
       </c>
       <c r="F10" s="25" t="s">
-        <v>788</v>
+        <v>790</v>
       </c>
       <c r="G10" s="25"/>
       <c r="H10" s="25"/>
@@ -28301,10 +28322,10 @@
     </row>
     <row r="11" s="10" customFormat="1" ht="41" customHeight="1" spans="1:15">
       <c r="A11" s="18" t="s">
-        <v>793</v>
+        <v>795</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>794</v>
+        <v>796</v>
       </c>
       <c r="C11" s="28" t="s">
         <v>35</v>
@@ -28313,10 +28334,10 @@
         <v>263</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="F11" s="29" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="G11" s="25"/>
       <c r="H11" s="25"/>
@@ -28338,7 +28359,7 @@
         <v>536</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="F12" s="26"/>
       <c r="G12" s="25"/>
@@ -28354,7 +28375,7 @@
     <row r="13" s="10" customFormat="1" ht="41" customHeight="1" spans="1:15">
       <c r="A13" s="18"/>
       <c r="B13" s="19" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="C13" s="24" t="s">
         <v>5</v>
@@ -28363,10 +28384,10 @@
         <v>471</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="F13" s="26" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="G13" s="25"/>
       <c r="H13" s="25"/>
@@ -28381,7 +28402,7 @@
     <row r="14" s="10" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A14" s="18"/>
       <c r="B14" s="19" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="C14" s="24" t="s">
         <v>35</v>
@@ -28390,11 +28411,11 @@
         <v>197</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="F14" s="25"/>
       <c r="G14" s="25" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="H14" s="25"/>
       <c r="I14" s="25"/>
@@ -28408,7 +28429,7 @@
     <row r="15" s="10" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A15" s="18"/>
       <c r="B15" s="19" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="C15" s="24" t="s">
         <v>5</v>
@@ -28417,10 +28438,10 @@
         <v>471</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="G15" s="25"/>
       <c r="H15" s="25"/>
@@ -28442,10 +28463,10 @@
         <v>447</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="F16" s="26" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
       <c r="G16" s="25"/>
       <c r="H16" s="25"/>
@@ -28460,7 +28481,7 @@
     <row r="17" s="10" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A17" s="18"/>
       <c r="B17" s="19" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
       <c r="C17" s="39" t="s">
         <v>5</v>
@@ -28469,10 +28490,10 @@
         <v>49</v>
       </c>
       <c r="E17" s="40" t="s">
-        <v>792</v>
+        <v>794</v>
       </c>
       <c r="F17" s="40" t="s">
-        <v>788</v>
+        <v>790</v>
       </c>
       <c r="G17" s="25"/>
       <c r="H17" s="25"/>
@@ -28486,10 +28507,10 @@
     </row>
     <row r="18" s="10" customFormat="1" ht="51" customHeight="1" spans="1:15">
       <c r="A18" s="18" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="C18" s="24" t="s">
         <v>5</v>
@@ -28498,10 +28519,10 @@
         <v>471</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="F18" s="26" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="G18" s="41"/>
       <c r="H18" s="29"/>
@@ -28516,7 +28537,7 @@
     <row r="19" s="10" customFormat="1" ht="18" customHeight="1" spans="1:15">
       <c r="A19" s="18"/>
       <c r="B19" s="38" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="C19" s="28" t="s">
         <v>35</v>
@@ -28525,11 +28546,11 @@
         <v>197</v>
       </c>
       <c r="E19" s="29" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="F19" s="29"/>
       <c r="G19" s="29" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="H19" s="29"/>
       <c r="I19" s="29"/>
@@ -28550,10 +28571,10 @@
         <v>447</v>
       </c>
       <c r="E20" s="29" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="F20" s="26" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="G20" s="25"/>
       <c r="H20" s="29"/>
@@ -28568,7 +28589,7 @@
     <row r="21" s="10" customFormat="1" ht="46" customHeight="1" spans="1:15">
       <c r="A21" s="18"/>
       <c r="B21" s="38" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
       <c r="C21" s="28" t="s">
         <v>35</v>
@@ -28577,7 +28598,7 @@
         <v>107</v>
       </c>
       <c r="E21" s="29" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="F21" s="29"/>
       <c r="G21" s="29"/>
@@ -28592,10 +28613,10 @@
     </row>
     <row r="22" s="10" customFormat="1" ht="46" customHeight="1" spans="1:15">
       <c r="A22" s="18" t="s">
-        <v>801</v>
+        <v>803</v>
       </c>
       <c r="B22" s="42" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
       <c r="C22" s="28" t="s">
         <v>35</v>
@@ -28604,10 +28625,10 @@
         <v>263</v>
       </c>
       <c r="E22" s="29" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="F22" s="29" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="G22" s="29"/>
       <c r="H22" s="29"/>
@@ -28621,7 +28642,7 @@
     </row>
     <row r="23" s="10" customFormat="1" ht="23" customHeight="1" spans="2:15">
       <c r="B23" s="19" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="C23" s="24" t="s">
         <v>5</v>
@@ -28630,10 +28651,10 @@
         <v>471</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="F23" s="26" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="G23" s="41"/>
       <c r="H23" s="25"/>
@@ -28648,7 +28669,7 @@
     <row r="24" s="10" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A24" s="18"/>
       <c r="B24" s="38" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
       <c r="C24" s="28" t="s">
         <v>35</v>
@@ -28657,11 +28678,11 @@
         <v>356</v>
       </c>
       <c r="E24" s="29" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="F24" s="29"/>
       <c r="G24" s="29" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="H24" s="25"/>
       <c r="I24" s="25"/>
@@ -28682,10 +28703,10 @@
         <v>447</v>
       </c>
       <c r="E25" s="29" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="F25" s="26" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="G25" s="25"/>
       <c r="H25" s="25"/>
@@ -28699,10 +28720,10 @@
     </row>
     <row r="26" s="10" customFormat="1" ht="53" customHeight="1" spans="1:15">
       <c r="A26" s="18" t="s">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="C26" s="24" t="s">
         <v>5</v>
@@ -28711,10 +28732,10 @@
         <v>471</v>
       </c>
       <c r="E26" s="25" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="F26" s="26" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="G26" s="41"/>
       <c r="H26" s="25"/>
@@ -28729,7 +28750,7 @@
     <row r="27" s="10" customFormat="1" ht="53" customHeight="1" spans="1:15">
       <c r="A27" s="18"/>
       <c r="B27" s="38" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="C27" s="28" t="s">
         <v>35</v>
@@ -28738,11 +28759,11 @@
         <v>197</v>
       </c>
       <c r="E27" s="29" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="F27" s="29"/>
       <c r="G27" s="29" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="H27" s="25"/>
       <c r="I27" s="25"/>
@@ -28763,10 +28784,10 @@
         <v>447</v>
       </c>
       <c r="E28" s="29" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="F28" s="26" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="G28" s="25"/>
       <c r="H28" s="25"/>
@@ -28781,7 +28802,7 @@
     <row r="29" s="10" customFormat="1" ht="53" customHeight="1" spans="1:15">
       <c r="A29" s="18"/>
       <c r="B29" s="38" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
       <c r="C29" s="28" t="s">
         <v>35</v>
@@ -28790,7 +28811,7 @@
         <v>107</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="F29" s="26"/>
       <c r="G29" s="41"/>
@@ -28805,10 +28826,10 @@
     </row>
     <row r="30" s="10" customFormat="1" ht="53" customHeight="1" spans="1:15">
       <c r="A30" s="18" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="C30" s="24" t="s">
         <v>5</v>
@@ -28817,10 +28838,10 @@
         <v>471</v>
       </c>
       <c r="E30" s="25" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="F30" s="26" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="G30" s="41"/>
       <c r="H30" s="25"/>
@@ -28835,7 +28856,7 @@
     <row r="31" s="10" customFormat="1" ht="53" customHeight="1" spans="1:15">
       <c r="A31" s="18"/>
       <c r="B31" s="19" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="C31" s="24" t="s">
         <v>35</v>
@@ -28844,11 +28865,11 @@
         <v>197</v>
       </c>
       <c r="E31" s="25" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="F31" s="43"/>
       <c r="G31" s="25" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="H31" s="25"/>
       <c r="I31" s="25"/>
@@ -28869,10 +28890,10 @@
         <v>447</v>
       </c>
       <c r="E32" s="25" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="F32" s="43" t="s">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="G32" s="41"/>
       <c r="H32" s="25"/>
@@ -28886,10 +28907,10 @@
     </row>
     <row r="33" s="10" customFormat="1" ht="44" customHeight="1" spans="1:15">
       <c r="A33" s="18" t="s">
-        <v>808</v>
+        <v>810</v>
       </c>
       <c r="B33" s="38" t="s">
-        <v>794</v>
+        <v>796</v>
       </c>
       <c r="C33" s="28" t="s">
         <v>35</v>
@@ -28898,10 +28919,10 @@
         <v>263</v>
       </c>
       <c r="E33" s="29" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="F33" s="29" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="G33" s="25"/>
       <c r="H33" s="25"/>
@@ -28915,7 +28936,7 @@
     </row>
     <row r="34" s="10" customFormat="1" ht="41" customHeight="1" spans="2:15">
       <c r="B34" s="19" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="C34" s="24" t="s">
         <v>5</v>
@@ -28924,10 +28945,10 @@
         <v>471</v>
       </c>
       <c r="E34" s="25" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="F34" s="26" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="G34" s="41"/>
       <c r="H34" s="25"/>
@@ -28942,7 +28963,7 @@
     <row r="35" s="10" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A35" s="18"/>
       <c r="B35" s="38" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="C35" s="28" t="s">
         <v>35</v>
@@ -28951,11 +28972,11 @@
         <v>197</v>
       </c>
       <c r="E35" s="29" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="F35" s="29"/>
       <c r="G35" s="29" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="H35" s="25"/>
       <c r="I35" s="25"/>
@@ -28976,10 +28997,10 @@
         <v>447</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="F36" s="26" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
       <c r="G36" s="25"/>
       <c r="H36" s="25"/>
@@ -28993,10 +29014,10 @@
     </row>
     <row r="37" s="10" customFormat="1" ht="73" customHeight="1" spans="1:15">
       <c r="A37" s="18" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="C37" s="24" t="s">
         <v>5</v>
@@ -29005,10 +29026,10 @@
         <v>471</v>
       </c>
       <c r="E37" s="25" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="F37" s="44" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="G37" s="41"/>
       <c r="H37" s="25"/>
@@ -29023,7 +29044,7 @@
     <row r="38" s="10" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A38" s="18"/>
       <c r="B38" s="38" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="C38" s="28" t="s">
         <v>35</v>
@@ -29032,11 +29053,11 @@
         <v>197</v>
       </c>
       <c r="E38" s="29" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="F38" s="29"/>
       <c r="G38" s="29" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="H38" s="25"/>
       <c r="I38" s="25"/>
@@ -29057,10 +29078,10 @@
         <v>447</v>
       </c>
       <c r="E39" s="29" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="F39" s="26" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="G39" s="25"/>
       <c r="H39" s="25"/>
@@ -29075,7 +29096,7 @@
     <row r="40" s="10" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A40" s="18"/>
       <c r="B40" s="38" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
       <c r="C40" s="28" t="s">
         <v>35</v>
@@ -29084,7 +29105,7 @@
         <v>107</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="F40" s="29"/>
       <c r="G40" s="29"/>
@@ -29099,10 +29120,10 @@
     </row>
     <row r="41" s="10" customFormat="1" ht="39" customHeight="1" spans="1:15">
       <c r="A41" s="18" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
       <c r="B41" s="42" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
       <c r="C41" s="28" t="s">
         <v>35</v>
@@ -29111,10 +29132,10 @@
         <v>263</v>
       </c>
       <c r="E41" s="29" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="F41" s="29" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="G41" s="29"/>
       <c r="H41" s="29"/>
@@ -29128,7 +29149,7 @@
     </row>
     <row r="42" s="10" customFormat="1" ht="42" customHeight="1" spans="2:15">
       <c r="B42" s="19" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="C42" s="24" t="s">
         <v>5</v>
@@ -29137,10 +29158,10 @@
         <v>471</v>
       </c>
       <c r="E42" s="25" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="F42" s="26" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="G42" s="41"/>
       <c r="H42" s="25"/>
@@ -29155,7 +29176,7 @@
     <row r="43" spans="1:10">
       <c r="A43" s="18"/>
       <c r="B43" s="38" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
       <c r="C43" s="28" t="s">
         <v>35</v>
@@ -29164,11 +29185,11 @@
         <v>356</v>
       </c>
       <c r="E43" s="29" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="F43" s="29"/>
       <c r="G43" s="29" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="H43" s="25"/>
       <c r="I43" s="25"/>
@@ -29184,10 +29205,10 @@
         <v>447</v>
       </c>
       <c r="E44" s="29" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="F44" s="26" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="G44" s="25"/>
       <c r="H44" s="25"/>
@@ -29196,10 +29217,10 @@
     </row>
     <row r="45" ht="42" spans="1:10">
       <c r="A45" s="18" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="C45" s="24" t="s">
         <v>5</v>
@@ -29208,10 +29229,10 @@
         <v>471</v>
       </c>
       <c r="E45" s="25" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="F45" s="45" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="G45" s="41"/>
       <c r="H45" s="25"/>
@@ -29221,7 +29242,7 @@
     <row r="46" spans="1:10">
       <c r="A46" s="18"/>
       <c r="B46" s="38" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="C46" s="28" t="s">
         <v>35</v>
@@ -29230,11 +29251,11 @@
         <v>197</v>
       </c>
       <c r="E46" s="29" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="F46" s="29"/>
       <c r="G46" s="29" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="H46" s="25"/>
       <c r="I46" s="25"/>
@@ -29250,10 +29271,10 @@
         <v>447</v>
       </c>
       <c r="E47" s="29" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="F47" s="26" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="G47" s="25"/>
       <c r="H47" s="25"/>
@@ -29262,10 +29283,10 @@
     </row>
     <row r="48" ht="56" spans="1:10">
       <c r="A48" s="18" t="s">
-        <v>813</v>
+        <v>815</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="C48" s="24" t="s">
         <v>5</v>
@@ -29274,10 +29295,10 @@
         <v>471</v>
       </c>
       <c r="E48" s="25" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="F48" s="45" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c r="G48" s="41"/>
       <c r="H48" s="25"/>
@@ -29287,7 +29308,7 @@
     <row r="49" spans="1:10">
       <c r="A49" s="18"/>
       <c r="B49" s="38" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="C49" s="28" t="s">
         <v>35</v>
@@ -29296,11 +29317,11 @@
         <v>197</v>
       </c>
       <c r="E49" s="29" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="F49" s="29"/>
       <c r="G49" s="29" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="H49" s="25"/>
       <c r="I49" s="25"/>
@@ -29316,10 +29337,10 @@
         <v>447</v>
       </c>
       <c r="E50" s="29" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="F50" s="26" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="G50" s="25"/>
       <c r="H50" s="25"/>
@@ -29328,10 +29349,10 @@
     </row>
     <row r="51" ht="57" customHeight="1" spans="1:10">
       <c r="A51" s="18" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="C51" s="24" t="s">
         <v>5</v>
@@ -29340,10 +29361,10 @@
         <v>471</v>
       </c>
       <c r="E51" s="25" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="F51" s="43" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
       <c r="G51" s="41"/>
       <c r="H51" s="25"/>
@@ -29353,7 +29374,7 @@
     <row r="52" spans="1:10">
       <c r="A52" s="18"/>
       <c r="B52" s="38" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="C52" s="28" t="s">
         <v>35</v>
@@ -29362,11 +29383,11 @@
         <v>197</v>
       </c>
       <c r="E52" s="29" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="F52" s="29"/>
       <c r="G52" s="29" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="H52" s="25"/>
       <c r="I52" s="25"/>
@@ -29382,10 +29403,10 @@
         <v>447</v>
       </c>
       <c r="E53" s="29" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="F53" s="26" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
       <c r="G53" s="25"/>
       <c r="H53" s="25"/>
@@ -29394,10 +29415,10 @@
     </row>
     <row r="54" ht="58" customHeight="1" spans="1:10">
       <c r="A54" s="18" t="s">
-        <v>817</v>
+        <v>819</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="C54" s="24" t="s">
         <v>5</v>
@@ -29406,10 +29427,10 @@
         <v>471</v>
       </c>
       <c r="E54" s="25" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="F54" s="43" t="s">
-        <v>818</v>
+        <v>820</v>
       </c>
       <c r="G54" s="41"/>
       <c r="H54" s="25"/>
@@ -29419,7 +29440,7 @@
     <row r="55" ht="33" customHeight="1" spans="1:10">
       <c r="A55" s="18"/>
       <c r="B55" s="38" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="C55" s="28" t="s">
         <v>35</v>
@@ -29428,11 +29449,11 @@
         <v>197</v>
       </c>
       <c r="E55" s="29" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="F55" s="29"/>
       <c r="G55" s="29" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="H55" s="25"/>
       <c r="I55" s="25"/>
@@ -29448,10 +29469,10 @@
         <v>447</v>
       </c>
       <c r="E56" s="29" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="F56" s="26" t="s">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="G56" s="25"/>
       <c r="H56" s="25"/>
@@ -29460,10 +29481,10 @@
     </row>
     <row r="57" ht="70" spans="1:10">
       <c r="A57" s="18" t="s">
-        <v>819</v>
+        <v>821</v>
       </c>
       <c r="B57" s="19" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="C57" s="24" t="s">
         <v>5</v>
@@ -29472,10 +29493,10 @@
         <v>471</v>
       </c>
       <c r="E57" s="25" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="F57" s="43" t="s">
-        <v>820</v>
+        <v>822</v>
       </c>
       <c r="G57" s="41"/>
       <c r="H57" s="25"/>
@@ -29485,7 +29506,7 @@
     <row r="58" spans="1:10">
       <c r="A58" s="18"/>
       <c r="B58" s="38" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="C58" s="28" t="s">
         <v>35</v>
@@ -29494,11 +29515,11 @@
         <v>197</v>
       </c>
       <c r="E58" s="29" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="F58" s="29"/>
       <c r="G58" s="29" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="H58" s="25"/>
       <c r="I58" s="25"/>
@@ -29514,10 +29535,10 @@
         <v>447</v>
       </c>
       <c r="E59" s="29" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="F59" s="26" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c r="G59" s="25"/>
       <c r="H59" s="25"/>
@@ -29527,7 +29548,7 @@
     <row r="60" spans="1:10">
       <c r="A60" s="46"/>
       <c r="B60" s="38" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
       <c r="C60" s="28" t="s">
         <v>35</v>
@@ -29536,7 +29557,7 @@
         <v>107</v>
       </c>
       <c r="E60" s="29" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="F60" s="47"/>
       <c r="G60" s="29"/>
@@ -29603,8 +29624,8 @@
   <sheetPr/>
   <dimension ref="A1:O107"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
@@ -29661,7 +29682,7 @@
     </row>
     <row r="2" ht="93" customHeight="1" spans="1:15">
       <c r="A2" s="14" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
@@ -29671,7 +29692,7 @@
       <c r="G2" s="16"/>
       <c r="H2" s="16"/>
       <c r="I2" s="17" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="J2" s="31"/>
       <c r="K2" s="21"/>
@@ -29744,10 +29765,10 @@
     </row>
     <row r="5" ht="23" customHeight="1" spans="1:15">
       <c r="A5" s="27" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="C5" s="24" t="s">
         <v>5</v>
@@ -29756,10 +29777,10 @@
         <v>471</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="G5" s="25"/>
       <c r="H5" s="25"/>
@@ -29781,10 +29802,10 @@
         <v>263</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="F6" s="29" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="G6" s="25"/>
       <c r="H6" s="25"/>
@@ -29799,7 +29820,7 @@
     <row r="7" ht="32" customHeight="1" spans="1:15">
       <c r="A7" s="18"/>
       <c r="B7" s="19" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="C7" s="24" t="s">
         <v>35</v>
@@ -29808,10 +29829,10 @@
         <v>263</v>
       </c>
       <c r="E7" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
       <c r="F7" t="s">
-        <v>825</v>
+        <v>827</v>
       </c>
       <c r="G7" s="25"/>
       <c r="H7" s="25"/>
@@ -29826,7 +29847,7 @@
     <row r="8" ht="23" customHeight="1" spans="1:15">
       <c r="A8" s="18"/>
       <c r="B8" s="19" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="C8" s="24" t="s">
         <v>35</v>
@@ -29835,16 +29856,16 @@
         <v>395</v>
       </c>
       <c r="E8" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>826</v>
+        <v>828</v>
       </c>
       <c r="G8" s="25" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="H8" s="25" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="I8" s="25"/>
       <c r="J8" s="26"/>
@@ -29864,7 +29885,7 @@
         <v>536</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>790</v>
+        <v>792</v>
       </c>
       <c r="F9" s="25"/>
       <c r="G9" s="25"/>
@@ -29880,7 +29901,7 @@
     <row r="10" ht="23" customHeight="1" spans="1:15">
       <c r="A10" s="18"/>
       <c r="B10" s="19" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
       <c r="C10" s="24" t="s">
         <v>5</v>
@@ -29889,10 +29910,10 @@
         <v>471</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="F10" s="25" t="s">
-        <v>828</v>
+        <v>830</v>
       </c>
       <c r="G10" s="25"/>
       <c r="H10" s="25"/>
@@ -29914,10 +29935,10 @@
         <v>447</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="F11" s="26" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
       <c r="G11" s="25"/>
       <c r="H11" s="25"/>
@@ -29939,10 +29960,10 @@
         <v>49</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>787</v>
+        <v>789</v>
       </c>
       <c r="F12" s="25" t="s">
-        <v>788</v>
+        <v>790</v>
       </c>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
@@ -29957,7 +29978,7 @@
     <row r="13" ht="23" customHeight="1" spans="1:15">
       <c r="A13" s="18"/>
       <c r="B13" s="19" t="s">
-        <v>830</v>
+        <v>832</v>
       </c>
       <c r="C13" s="28" t="s">
         <v>35</v>
@@ -29966,7 +29987,7 @@
         <v>107</v>
       </c>
       <c r="E13" s="29" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="F13" s="25"/>
       <c r="G13" s="25"/>
@@ -31686,7 +31707,7 @@
     </row>
     <row r="2" ht="93" customHeight="1" spans="1:15">
       <c r="A2" s="14" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
@@ -31696,7 +31717,7 @@
       <c r="G2" s="16"/>
       <c r="H2" s="16"/>
       <c r="I2" s="17" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="J2" s="31"/>
       <c r="K2" s="21"/>
@@ -31769,10 +31790,10 @@
     </row>
     <row r="5" ht="46" customHeight="1" spans="1:15">
       <c r="A5" s="18" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
       <c r="C5" s="24" t="s">
         <v>5</v>
@@ -31781,10 +31802,10 @@
         <v>471</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="G5" s="25"/>
       <c r="H5" s="25"/>
@@ -31806,10 +31827,10 @@
         <v>263</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="F6" s="29" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="G6" s="25"/>
       <c r="H6" s="25"/>
@@ -31831,10 +31852,10 @@
         <v>263</v>
       </c>
       <c r="E7" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
       <c r="F7" t="s">
-        <v>825</v>
+        <v>827</v>
       </c>
       <c r="G7" s="25"/>
       <c r="H7" s="25"/>
@@ -31856,16 +31877,16 @@
         <v>395</v>
       </c>
       <c r="E8" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>826</v>
+        <v>828</v>
       </c>
       <c r="G8" s="25" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="H8" s="25" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="I8" s="25"/>
       <c r="J8" s="26"/>
@@ -31885,10 +31906,10 @@
         <v>447</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="F9" s="26" t="s">
-        <v>834</v>
+        <v>836</v>
       </c>
       <c r="G9" s="25"/>
       <c r="H9" s="25"/>
@@ -31903,7 +31924,7 @@
     <row r="10" ht="23" customHeight="1" spans="1:15">
       <c r="A10" s="18"/>
       <c r="B10" s="19" t="s">
-        <v>830</v>
+        <v>832</v>
       </c>
       <c r="C10" s="28" t="s">
         <v>35</v>
@@ -31912,7 +31933,7 @@
         <v>107</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="F10" s="25"/>
       <c r="G10" s="25"/>
@@ -31927,10 +31948,10 @@
     </row>
     <row r="11" ht="59" customHeight="1" spans="1:15">
       <c r="A11" s="18" t="s">
-        <v>835</v>
+        <v>837</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
       <c r="C11" s="24" t="s">
         <v>5</v>
@@ -31939,10 +31960,10 @@
         <v>471</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="F11" s="26" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
       <c r="G11" s="25"/>
       <c r="H11" s="25"/>
@@ -31964,10 +31985,10 @@
         <v>263</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="F12" s="29" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
@@ -31989,10 +32010,10 @@
         <v>263</v>
       </c>
       <c r="E13" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
       <c r="F13" t="s">
-        <v>825</v>
+        <v>827</v>
       </c>
       <c r="G13" s="25"/>
       <c r="H13" s="25"/>
@@ -32014,16 +32035,16 @@
         <v>395</v>
       </c>
       <c r="E14" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="F14" s="25" t="s">
-        <v>826</v>
+        <v>828</v>
       </c>
       <c r="G14" s="25" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="H14" s="25" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="I14" s="25"/>
       <c r="J14" s="26"/>
@@ -32043,10 +32064,10 @@
         <v>447</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="F15" s="26" t="s">
-        <v>834</v>
+        <v>836</v>
       </c>
       <c r="G15" s="25"/>
       <c r="H15" s="25"/>
@@ -32061,7 +32082,7 @@
     <row r="16" ht="23" customHeight="1" spans="1:15">
       <c r="A16" s="18"/>
       <c r="B16" s="19" t="s">
-        <v>830</v>
+        <v>832</v>
       </c>
       <c r="C16" s="28" t="s">
         <v>35</v>
@@ -32070,7 +32091,7 @@
         <v>107</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="F16" s="25"/>
       <c r="G16" s="25"/>
@@ -32085,10 +32106,10 @@
     </row>
     <row r="17" ht="56" customHeight="1" spans="1:15">
       <c r="A17" s="18" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
       <c r="C17" s="24" t="s">
         <v>5</v>
@@ -32097,10 +32118,10 @@
         <v>471</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="F17" s="26" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="G17" s="25"/>
       <c r="H17" s="25"/>
@@ -32122,10 +32143,10 @@
         <v>263</v>
       </c>
       <c r="E18" s="29" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="F18" s="29" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="G18" s="25"/>
       <c r="H18" s="25"/>
@@ -32147,10 +32168,10 @@
         <v>263</v>
       </c>
       <c r="E19" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
       <c r="F19" t="s">
-        <v>825</v>
+        <v>827</v>
       </c>
       <c r="G19" s="25"/>
       <c r="H19" s="25"/>
@@ -32172,16 +32193,16 @@
         <v>395</v>
       </c>
       <c r="E20" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="F20" s="30" t="s">
-        <v>826</v>
+        <v>828</v>
       </c>
       <c r="G20" s="25" t="s">
-        <v>838</v>
+        <v>840</v>
       </c>
       <c r="H20" s="25" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="I20" s="25"/>
       <c r="J20" s="26"/>
@@ -32201,10 +32222,10 @@
         <v>447</v>
       </c>
       <c r="E21" s="25" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="F21" s="26" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c r="G21" s="25"/>
       <c r="H21" s="25"/>
@@ -32219,7 +32240,7 @@
     <row r="22" ht="23" customHeight="1" spans="1:15">
       <c r="A22" s="18"/>
       <c r="B22" s="19" t="s">
-        <v>830</v>
+        <v>832</v>
       </c>
       <c r="C22" s="28" t="s">
         <v>35</v>
@@ -32228,7 +32249,7 @@
         <v>107</v>
       </c>
       <c r="E22" s="29" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="F22" s="25"/>
       <c r="G22" s="25"/>
@@ -32243,10 +32264,10 @@
     </row>
     <row r="23" ht="64" customHeight="1" spans="1:15">
       <c r="A23" s="18" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
       <c r="C23" s="24" t="s">
         <v>5</v>
@@ -32255,10 +32276,10 @@
         <v>471</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="F23" s="26" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="G23" s="25"/>
       <c r="H23" s="25"/>
@@ -32280,10 +32301,10 @@
         <v>263</v>
       </c>
       <c r="E24" s="29" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="F24" s="29" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="G24" s="25"/>
       <c r="H24" s="25"/>
@@ -32305,10 +32326,10 @@
         <v>263</v>
       </c>
       <c r="E25" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
       <c r="F25" t="s">
-        <v>825</v>
+        <v>827</v>
       </c>
       <c r="G25" s="25"/>
       <c r="H25" s="25"/>
@@ -32330,16 +32351,16 @@
         <v>395</v>
       </c>
       <c r="E26" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="F26" s="30" t="s">
-        <v>826</v>
+        <v>828</v>
       </c>
       <c r="G26" s="25" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="H26" s="25" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="I26" s="25"/>
       <c r="J26" s="26"/>
@@ -32359,10 +32380,10 @@
         <v>447</v>
       </c>
       <c r="E27" s="25" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="F27" s="26" t="s">
-        <v>834</v>
+        <v>836</v>
       </c>
       <c r="G27" s="25"/>
       <c r="H27" s="25"/>
@@ -32377,7 +32398,7 @@
     <row r="28" ht="23" customHeight="1" spans="1:15">
       <c r="A28" s="18"/>
       <c r="B28" s="19" t="s">
-        <v>830</v>
+        <v>832</v>
       </c>
       <c r="C28" s="28" t="s">
         <v>35</v>
@@ -32386,7 +32407,7 @@
         <v>107</v>
       </c>
       <c r="E28" s="29" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="F28" s="25"/>
       <c r="G28" s="25"/>

</xml_diff>